<commit_message>
updated the code with error handlers
</commit_message>
<xml_diff>
--- a/Thesis/Chart Thesis 1.xlsx
+++ b/Thesis/Chart Thesis 1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20376"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D55A813-128E-4632-816A-0C84E44871FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A518688-1B0D-43EE-B0BA-16952DAC3257}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1715,9 +1715,6 @@
     <t>Electrolyser 3</t>
   </si>
   <si>
-    <t>Heat BalanceGgr.3</t>
-  </si>
-  <si>
     <t>Heat Balance Gr.2</t>
   </si>
   <si>
@@ -2253,6 +2250,9 @@
   </si>
   <si>
     <t>Chart Type 5</t>
+  </si>
+  <si>
+    <t>Heat Balance Gr.3</t>
   </si>
 </sst>
 </file>
@@ -4637,8 +4637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC8759-87D6-40A8-AF33-9EF83B136632}">
   <dimension ref="A1:U149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I25" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:U54"/>
+    <sheetView tabSelected="1" topLeftCell="H25" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4684,13 +4684,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>577</v>
+      </c>
+      <c r="I1" t="s">
+        <v>576</v>
+      </c>
+      <c r="J1" t="s">
         <v>578</v>
-      </c>
-      <c r="I1" t="s">
-        <v>577</v>
-      </c>
-      <c r="J1" t="s">
-        <v>579</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
@@ -4705,10 +4705,10 @@
         <v>440</v>
       </c>
       <c r="O1" t="s">
+        <v>737</v>
+      </c>
+      <c r="P1" t="s">
         <v>738</v>
-      </c>
-      <c r="P1" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -4725,20 +4725,20 @@
         <v>9</v>
       </c>
       <c r="E2" t="str">
-        <f>TRIM(C2) &amp;" " &amp; TRIM(D2)</f>
+        <f t="shared" ref="E2:E33" si="0">TRIM(C2) &amp;" " &amp; TRIM(D2)</f>
         <v>Electr. Demand</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>581</v>
-      </c>
       <c r="J2" s="10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="K2" t="s">
         <v>11</v>
@@ -4761,7 +4761,7 @@
         <v>0001_Electr. Demand</v>
       </c>
       <c r="Q2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="R2" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q2,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q2,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
@@ -4790,20 +4790,20 @@
         <v>13</v>
       </c>
       <c r="E3" t="str">
-        <f>TRIM(C3) &amp;" " &amp; TRIM(D3)</f>
+        <f t="shared" si="0"/>
         <v>Elec.dem Cooling</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="K3" t="s">
         <v>11</v>
@@ -4833,11 +4833,11 @@
         <v>0005</v>
       </c>
       <c r="T3" t="str">
-        <f t="shared" ref="T3:T54" si="0">"['"&amp;Q3&amp;"','"&amp;R3&amp;"']"</f>
+        <f t="shared" ref="T3:T54" si="1">"['"&amp;Q3&amp;"','"&amp;R3&amp;"']"</f>
         <v>['Boiler 1','0005']</v>
       </c>
       <c r="U3" t="str">
-        <f t="shared" ref="U3:U54" si="1">"'"&amp;Q3&amp;"':'"&amp;R3&amp;"',"</f>
+        <f t="shared" ref="U3:U54" si="2">"'"&amp;Q3&amp;"':'"&amp;R3&amp;"',"</f>
         <v>'Boiler 1':'0005',</v>
       </c>
     </row>
@@ -4855,20 +4855,20 @@
         <v>16</v>
       </c>
       <c r="E4" t="str">
-        <f>TRIM(C4) &amp;" " &amp; TRIM(D4)</f>
+        <f t="shared" si="0"/>
         <v>Fixed Exp/Imp</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="K4" t="s">
         <v>11</v>
@@ -4898,11 +4898,11 @@
         <v>0008</v>
       </c>
       <c r="T4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Boiler 2','0008']</v>
       </c>
       <c r="U4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Boiler 2':'0008',</v>
       </c>
     </row>
@@ -4920,20 +4920,20 @@
         <v>9</v>
       </c>
       <c r="E5" t="str">
-        <f>TRIM(C5) &amp;" " &amp; TRIM(D5)</f>
+        <f t="shared" si="0"/>
         <v>DH Demand</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="K5" t="s">
         <v>11</v>
@@ -4963,11 +4963,11 @@
         <v>0015</v>
       </c>
       <c r="T5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Boiler 3','0015']</v>
       </c>
       <c r="U5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Boiler 3':'0015',</v>
       </c>
     </row>
@@ -4985,20 +4985,20 @@
         <v>21</v>
       </c>
       <c r="E6" t="str">
-        <f>TRIM(C6) &amp;" " &amp; TRIM(D6)</f>
+        <f t="shared" si="0"/>
         <v>Wind Electr.</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="K6" t="s">
         <v>11</v>
@@ -5021,18 +5021,18 @@
         <v>0101_Wind Electr.</v>
       </c>
       <c r="Q6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="R6" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q6,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q6,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0006</v>
       </c>
       <c r="T6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Combined Heat &amp; Power 2','0006']</v>
       </c>
       <c r="U6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Combined Heat &amp; Power 2':'0006',</v>
       </c>
     </row>
@@ -5050,20 +5050,20 @@
         <v>21</v>
       </c>
       <c r="E7" t="str">
-        <f>TRIM(C7) &amp;" " &amp; TRIM(D7)</f>
+        <f t="shared" si="0"/>
         <v>Offshore Electr.</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>581</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>582</v>
-      </c>
       <c r="J7" s="10" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="K7" t="s">
         <v>11</v>
@@ -5086,18 +5086,18 @@
         <v>0102_Offshore Electr.</v>
       </c>
       <c r="Q7" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="R7" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q7,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q7,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0023</v>
       </c>
       <c r="T7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Combined Heat &amp; Power Electricity Production','0023']</v>
       </c>
       <c r="U7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Combined Heat &amp; Power Electricity Production':'0023',</v>
       </c>
     </row>
@@ -5115,20 +5115,20 @@
         <v>21</v>
       </c>
       <c r="E8" t="str">
-        <f>TRIM(C8) &amp;" " &amp; TRIM(D8)</f>
+        <f t="shared" si="0"/>
         <v>PV Electr.</v>
       </c>
       <c r="G8" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="K8" t="s">
         <v>11</v>
@@ -5158,11 +5158,11 @@
         <v>0013</v>
       </c>
       <c r="T8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Combined Heat and Power 3','0013']</v>
       </c>
       <c r="U8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Combined Heat and Power 3':'0013',</v>
       </c>
     </row>
@@ -5180,20 +5180,20 @@
         <v>21</v>
       </c>
       <c r="E9" t="str">
-        <f>TRIM(C9) &amp;" " &amp; TRIM(D9)</f>
+        <f t="shared" si="0"/>
         <v>CSP Electr.</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="K9" t="s">
         <v>11</v>
@@ -5216,18 +5216,18 @@
         <v>0104_CSP Electr.</v>
       </c>
       <c r="Q9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="R9" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q9,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q9,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0022</v>
       </c>
       <c r="T9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Combined Steam &amp; Heat Electricity Production','0022']</v>
       </c>
       <c r="U9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Combined Steam &amp; Heat Electricity Production':'0022',</v>
       </c>
     </row>
@@ -5245,20 +5245,20 @@
         <v>21</v>
       </c>
       <c r="E10" t="str">
-        <f>TRIM(C10) &amp;" " &amp; TRIM(D10)</f>
+        <f t="shared" si="0"/>
         <v>River Electr.</v>
       </c>
       <c r="G10" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="K10" t="s">
         <v>11</v>
@@ -5288,11 +5288,11 @@
         <v>0400</v>
       </c>
       <c r="T10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Combined Steam &amp; Heat Production','0400']</v>
       </c>
       <c r="U10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Combined Steam &amp; Heat Production':'0400',</v>
       </c>
     </row>
@@ -5310,20 +5310,20 @@
         <v>21</v>
       </c>
       <c r="E11" t="str">
-        <f>TRIM(C11) &amp;" " &amp; TRIM(D11)</f>
+        <f t="shared" si="0"/>
         <v>Wave Electr.</v>
       </c>
       <c r="G11" t="s">
         <v>22</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="K11" t="s">
         <v>11</v>
@@ -5346,18 +5346,18 @@
         <v>0106_Wave Electr.</v>
       </c>
       <c r="Q11" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="R11" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q11,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q11,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0027</v>
       </c>
       <c r="T11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Critical Electricity Excess Production','0027']</v>
       </c>
       <c r="U11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Critical Electricity Excess Production':'0027',</v>
       </c>
     </row>
@@ -5375,20 +5375,20 @@
         <v>21</v>
       </c>
       <c r="E12" t="str">
-        <f>TRIM(C12) &amp;" " &amp; TRIM(D12)</f>
+        <f t="shared" si="0"/>
         <v>Tidal Electr.</v>
       </c>
       <c r="G12" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="K12" t="s">
         <v>11</v>
@@ -5418,11 +5418,11 @@
         <v>2200</v>
       </c>
       <c r="T12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Desalination','2200']</v>
       </c>
       <c r="U12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Desalination':'2200',</v>
       </c>
     </row>
@@ -5440,20 +5440,20 @@
         <v>21</v>
       </c>
       <c r="E13" t="str">
-        <f>TRIM(C13) &amp;" " &amp; TRIM(D13)</f>
+        <f t="shared" si="0"/>
         <v>CSP2 Electr.</v>
       </c>
       <c r="G13" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="K13" t="s">
         <v>11</v>
@@ -5483,11 +5483,11 @@
         <v>2100</v>
       </c>
       <c r="T13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['District Cooling','2100']</v>
       </c>
       <c r="U13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'District Cooling':'2100',</v>
       </c>
     </row>
@@ -5505,20 +5505,20 @@
         <v>30</v>
       </c>
       <c r="E14" t="str">
-        <f>TRIM(C14) &amp;" " &amp; TRIM(D14)</f>
+        <f t="shared" si="0"/>
         <v>CSP2 Storage</v>
       </c>
       <c r="G14" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="K14" t="s">
         <v>11</v>
@@ -5548,11 +5548,11 @@
         <v>0004</v>
       </c>
       <c r="T14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['District Heat Demand','0004']</v>
       </c>
       <c r="U14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'District Heat Demand':'0004',</v>
       </c>
     </row>
@@ -5570,20 +5570,20 @@
         <v>31</v>
       </c>
       <c r="E15" t="str">
-        <f>TRIM(C15) &amp;" " &amp; TRIM(D15)</f>
+        <f t="shared" si="0"/>
         <v>CSP2 loss</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I15" s="10">
         <v>10</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K15" t="s">
         <v>11</v>
@@ -5613,11 +5613,11 @@
         <v>0001</v>
       </c>
       <c r="T15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Electricity Demand','0001']</v>
       </c>
       <c r="U15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Electricity Demand':'0001',</v>
       </c>
     </row>
@@ -5635,20 +5635,20 @@
         <v>21</v>
       </c>
       <c r="E16" t="str">
-        <f>TRIM(C16) &amp;" " &amp; TRIM(D16)</f>
+        <f t="shared" si="0"/>
         <v>Hydro Electr.</v>
       </c>
       <c r="G16" t="s">
         <v>33</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="K16" t="s">
         <v>11</v>
@@ -5678,11 +5678,11 @@
         <v>0002</v>
       </c>
       <c r="T16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Electricity Demand Cooling','0002']</v>
       </c>
       <c r="U16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Electricity Demand Cooling':'0002',</v>
       </c>
     </row>
@@ -5700,20 +5700,20 @@
         <v>34</v>
       </c>
       <c r="E17" t="str">
-        <f>TRIM(C17) &amp;" " &amp; TRIM(D17)</f>
+        <f t="shared" si="0"/>
         <v>Hydro pump</v>
       </c>
       <c r="G17" t="s">
         <v>33</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="K17" t="s">
         <v>11</v>
@@ -5736,18 +5736,18 @@
         <v>0202_Hydro pump</v>
       </c>
       <c r="Q17" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="R17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q17,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q17,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0009</v>
       </c>
       <c r="T17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Electricity Heat 2','0009']</v>
       </c>
       <c r="U17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Electricity Heat 2':'0009',</v>
       </c>
     </row>
@@ -5765,20 +5765,20 @@
         <v>35</v>
       </c>
       <c r="E18" t="str">
-        <f>TRIM(C18) &amp;" " &amp; TRIM(D18)</f>
+        <f t="shared" si="0"/>
         <v>Hydro storage</v>
       </c>
       <c r="G18" t="s">
         <v>33</v>
       </c>
       <c r="H18" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="I18" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>583</v>
-      </c>
       <c r="J18" s="10" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="K18" t="s">
         <v>11</v>
@@ -5801,18 +5801,18 @@
         <v>0203_Hydro storage</v>
       </c>
       <c r="Q18" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="R18" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q18,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q18,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0016</v>
       </c>
       <c r="T18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Electricity Heat 3','0016']</v>
       </c>
       <c r="U18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Electricity Heat 3':'0016',</v>
       </c>
     </row>
@@ -5830,20 +5830,20 @@
         <v>36</v>
       </c>
       <c r="E19" t="str">
-        <f>TRIM(C19) &amp;" " &amp; TRIM(D19)</f>
+        <f t="shared" si="0"/>
         <v>Hydro Wat-Sup</v>
       </c>
       <c r="G19" t="s">
         <v>33</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="K19" t="s">
         <v>11</v>
@@ -5873,11 +5873,11 @@
         <v>0010</v>
       </c>
       <c r="T19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Electrolyser 2','0010']</v>
       </c>
       <c r="U19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Electrolyser 2':'0010',</v>
       </c>
     </row>
@@ -5895,20 +5895,20 @@
         <v>37</v>
       </c>
       <c r="E20" t="str">
-        <f>TRIM(C20) &amp;" " &amp; TRIM(D20)</f>
+        <f t="shared" si="0"/>
         <v>Hydro Wat-Loss</v>
       </c>
       <c r="G20" t="s">
         <v>33</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="K20" t="s">
         <v>11</v>
@@ -5938,11 +5938,11 @@
         <v>0017</v>
       </c>
       <c r="T20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Electrolyser 3','0017']</v>
       </c>
       <c r="U20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Electrolyser 3':'0017',</v>
       </c>
     </row>
@@ -5960,20 +5960,20 @@
         <v>39</v>
       </c>
       <c r="E21" t="str">
-        <f>TRIM(C21) &amp;" " &amp; TRIM(D21)</f>
+        <f t="shared" si="0"/>
         <v>Solar Heat</v>
       </c>
       <c r="G21" t="s">
         <v>40</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="K21" t="s">
         <v>11</v>
@@ -5996,18 +5996,18 @@
         <v>0301_Solar Heat</v>
       </c>
       <c r="Q21" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="R21" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q21,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q21,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>1100</v>
       </c>
       <c r="T21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Electrolyser Gr.2','1100']</v>
       </c>
       <c r="U21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Electrolyser Gr.2':'1100',</v>
       </c>
     </row>
@@ -6025,20 +6025,20 @@
         <v>39</v>
       </c>
       <c r="E22" t="str">
-        <f>TRIM(C22) &amp;" " &amp; TRIM(D22)</f>
+        <f t="shared" si="0"/>
         <v>CSHP 1 Heat</v>
       </c>
       <c r="G22" t="s">
         <v>42</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="K22" t="s">
         <v>11</v>
@@ -6061,18 +6061,18 @@
         <v>0401_CSHP 1 Heat</v>
       </c>
       <c r="Q22" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="R22" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q22,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q22,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>1200</v>
       </c>
       <c r="T22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Electrolyser Gr.3','1200']</v>
       </c>
       <c r="U22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Electrolyser Gr.3':'1200',</v>
       </c>
     </row>
@@ -6090,20 +6090,20 @@
         <v>39</v>
       </c>
       <c r="E23" t="str">
-        <f>TRIM(C23) &amp;" " &amp; TRIM(D23)</f>
+        <f t="shared" si="0"/>
         <v>Waste 1 Heat</v>
       </c>
       <c r="G23" t="s">
         <v>42</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="K23" t="s">
         <v>11</v>
@@ -6133,11 +6133,11 @@
         <v>1300</v>
       </c>
       <c r="T23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['EV &amp; V2G (Transport)','1300']</v>
       </c>
       <c r="U23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'EV &amp; V2G (Transport)':'1300',</v>
       </c>
     </row>
@@ -6155,20 +6155,20 @@
         <v>39</v>
       </c>
       <c r="E24" t="str">
-        <f>TRIM(C24) &amp;" " &amp; TRIM(D24)</f>
+        <f t="shared" si="0"/>
         <v>Boiler 1 Heat</v>
       </c>
       <c r="F24" t="s">
         <v>44</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="K24" t="s">
         <v>11</v>
@@ -6182,18 +6182,18 @@
         <v>0005_Boiler 1 Heat</v>
       </c>
       <c r="Q24" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="R24" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q24,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q24,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0026</v>
       </c>
       <c r="T24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Exorted Electricity','0026']</v>
       </c>
       <c r="U24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Exorted Electricity':'0026',</v>
       </c>
     </row>
@@ -6211,20 +6211,20 @@
         <v>46</v>
       </c>
       <c r="E25" t="str">
-        <f>TRIM(C25) &amp;" " &amp; TRIM(D25)</f>
+        <f t="shared" si="0"/>
         <v>Solar 1 Heat</v>
       </c>
       <c r="G25" t="s">
         <v>40</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="K25" t="s">
         <v>11</v>
@@ -6247,18 +6247,18 @@
         <v>0302_Solar 1 Heat</v>
       </c>
       <c r="Q25" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="R25" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q25,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q25,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0028</v>
       </c>
       <c r="T25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Exportable Electricity Excess Production','0028']</v>
       </c>
       <c r="U25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Exportable Electricity Excess Production':'0028',</v>
       </c>
     </row>
@@ -6276,20 +6276,20 @@
         <v>39</v>
       </c>
       <c r="E26" t="str">
-        <f>TRIM(C26) &amp;" " &amp; TRIM(D26)</f>
+        <f t="shared" si="0"/>
         <v>Sol1 Str Heat</v>
       </c>
       <c r="G26" t="s">
         <v>40</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K26" t="s">
         <v>11</v>
@@ -6319,11 +6319,11 @@
         <v>1600</v>
       </c>
       <c r="T26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Exports Payment','1600']</v>
       </c>
       <c r="U26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Exports Payment':'1600',</v>
       </c>
     </row>
@@ -6341,20 +6341,20 @@
         <v>39</v>
       </c>
       <c r="E27" t="str">
-        <f>TRIM(C27) &amp;" " &amp; TRIM(D27)</f>
+        <f t="shared" si="0"/>
         <v>CSHP 2 Heat</v>
       </c>
       <c r="G27" t="s">
         <v>42</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K27" t="s">
         <v>11</v>
@@ -6384,11 +6384,11 @@
         <v>0003</v>
       </c>
       <c r="T27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Fixed Export / Import','0003']</v>
       </c>
       <c r="U27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Fixed Export / Import':'0003',</v>
       </c>
     </row>
@@ -6406,20 +6406,20 @@
         <v>39</v>
       </c>
       <c r="E28" t="str">
-        <f>TRIM(C28) &amp;" " &amp; TRIM(D28)</f>
+        <f t="shared" si="0"/>
         <v>Waste 2 Heat</v>
       </c>
       <c r="G28" t="s">
         <v>42</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="K28" t="s">
         <v>11</v>
@@ -6449,11 +6449,11 @@
         <v>0020</v>
       </c>
       <c r="T28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Flexible Electricity demand','0020']</v>
       </c>
       <c r="U28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Flexible Electricity demand':'0020',</v>
       </c>
     </row>
@@ -6471,20 +6471,20 @@
         <v>39</v>
       </c>
       <c r="E29" t="str">
-        <f>TRIM(C29) &amp;" " &amp; TRIM(D29)</f>
+        <f t="shared" si="0"/>
         <v>Geoth 2 Heat</v>
       </c>
       <c r="G29" t="s">
         <v>51</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K29" t="s">
         <v>11</v>
@@ -6514,11 +6514,11 @@
         <v>2300</v>
       </c>
       <c r="T29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Gas Grid Demand &amp; Balance','2300']</v>
       </c>
       <c r="U29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Gas Grid Demand &amp; Balance':'2300',</v>
       </c>
     </row>
@@ -6536,20 +6536,20 @@
         <v>52</v>
       </c>
       <c r="E30" t="str">
-        <f>TRIM(C30) &amp;" " &amp; TRIM(D30)</f>
+        <f t="shared" si="0"/>
         <v>Geoth 2 Steam</v>
       </c>
       <c r="G30" t="s">
         <v>51</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K30" t="s">
         <v>11</v>
@@ -6579,11 +6579,11 @@
         <v>0500</v>
       </c>
       <c r="T30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Geothermal Heat Production','0500']</v>
       </c>
       <c r="U30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Geothermal Heat Production':'0500',</v>
       </c>
     </row>
@@ -6601,20 +6601,20 @@
         <v>53</v>
       </c>
       <c r="E31" t="str">
-        <f>TRIM(C31) &amp;" " &amp; TRIM(D31)</f>
+        <f t="shared" si="0"/>
         <v>Geoth 2 Storage</v>
       </c>
       <c r="G31" t="s">
         <v>51</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="K31" t="s">
         <v>11</v>
@@ -6637,18 +6637,18 @@
         <v>0503_Geoth 2 Storage</v>
       </c>
       <c r="Q31" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="R31" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q31,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q31,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0012</v>
       </c>
       <c r="T31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Heat Balance Gr.2','0012']</v>
       </c>
       <c r="U31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Heat Balance Gr.2':'0012',</v>
       </c>
     </row>
@@ -6666,20 +6666,20 @@
         <v>39</v>
       </c>
       <c r="E32" t="str">
-        <f>TRIM(C32) &amp;" " &amp; TRIM(D32)</f>
+        <f t="shared" si="0"/>
         <v>CHP 2 Heat</v>
       </c>
       <c r="F32" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="K32" t="s">
         <v>11</v>
@@ -6702,19 +6702,19 @@
         <v>0006_CHP 2 Heat</v>
       </c>
       <c r="Q32" t="s">
-        <v>560</v>
+        <v>739</v>
       </c>
       <c r="R32" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q32,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q32,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0019</v>
       </c>
       <c r="T32" t="str">
-        <f t="shared" si="0"/>
-        <v>['Heat BalanceGgr.3','0019']</v>
+        <f t="shared" si="1"/>
+        <v>['Heat Balance Gr.3','0019']</v>
       </c>
       <c r="U32" t="str">
-        <f t="shared" si="1"/>
-        <v>'Heat BalanceGgr.3':'0019',</v>
+        <f t="shared" si="2"/>
+        <v>'Heat Balance Gr.3':'0019',</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -6731,20 +6731,20 @@
         <v>39</v>
       </c>
       <c r="E33" t="str">
-        <f>TRIM(C33) &amp;" " &amp; TRIM(D33)</f>
+        <f t="shared" si="0"/>
         <v>HP 2 Heat</v>
       </c>
       <c r="F33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="K33" t="s">
         <v>11</v>
@@ -6767,18 +6767,18 @@
         <v>0007_HP 2 Heat</v>
       </c>
       <c r="Q33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="R33" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q33,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q33,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0007</v>
       </c>
       <c r="T33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Heat Pump 2','0007']</v>
       </c>
       <c r="U33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Heat Pump 2':'0007',</v>
       </c>
     </row>
@@ -6796,20 +6796,20 @@
         <v>39</v>
       </c>
       <c r="E34" t="str">
-        <f>TRIM(C34) &amp;" " &amp; TRIM(D34)</f>
+        <f t="shared" ref="E34:E65" si="3">TRIM(C34) &amp;" " &amp; TRIM(D34)</f>
         <v>Boiler 2 Heat</v>
       </c>
       <c r="F34" t="s">
         <v>56</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K34" t="s">
         <v>11</v>
@@ -6839,11 +6839,11 @@
         <v>0014</v>
       </c>
       <c r="T34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Heat Pump 3','0014']</v>
       </c>
       <c r="U34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Heat Pump 3':'0014',</v>
       </c>
     </row>
@@ -6861,20 +6861,20 @@
         <v>39</v>
       </c>
       <c r="E35" t="str">
-        <f>TRIM(C35) &amp;" " &amp; TRIM(D35)</f>
+        <f t="shared" si="3"/>
         <v>EH 2 Heat</v>
       </c>
       <c r="F35" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K35" t="s">
         <v>11</v>
@@ -6897,18 +6897,18 @@
         <v>0009_EH 2 Heat</v>
       </c>
       <c r="Q35" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="R35" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q35,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q35,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0021</v>
       </c>
       <c r="T35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Heat Pump Electricity Production','0021']</v>
       </c>
       <c r="U35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Heat Pump Electricity Production':'0021',</v>
       </c>
     </row>
@@ -6926,20 +6926,20 @@
         <v>39</v>
       </c>
       <c r="E36" t="str">
-        <f>TRIM(C36) &amp;" " &amp; TRIM(D36)</f>
+        <f t="shared" si="3"/>
         <v>ELT 2 Heat</v>
       </c>
       <c r="F36" t="s">
         <v>556</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I36" s="10">
         <v>10</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="K36" t="s">
         <v>11</v>
@@ -6969,11 +6969,11 @@
         <v>0200</v>
       </c>
       <c r="T36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Hydrolic Powers','0200']</v>
       </c>
       <c r="U36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Hydrolic Powers':'0200',</v>
       </c>
     </row>
@@ -6991,20 +6991,20 @@
         <v>39</v>
       </c>
       <c r="E37" t="str">
-        <f>TRIM(C37) &amp;" " &amp; TRIM(D37)</f>
+        <f t="shared" si="3"/>
         <v>Solar2 Heat</v>
       </c>
       <c r="G37" t="s">
         <v>40</v>
       </c>
       <c r="H37" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>583</v>
       </c>
-      <c r="I37" s="9" t="s">
-        <v>584</v>
-      </c>
       <c r="J37" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="K37" t="s">
         <v>11</v>
@@ -7034,11 +7034,11 @@
         <v>0029</v>
       </c>
       <c r="T37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Import Payment','0029']</v>
       </c>
       <c r="U37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Import Payment':'0029',</v>
       </c>
     </row>
@@ -7056,20 +7056,20 @@
         <v>39</v>
       </c>
       <c r="E38" t="str">
-        <f>TRIM(C38) &amp;" " &amp; TRIM(D38)</f>
+        <f t="shared" si="3"/>
         <v>Sol2 Str Heat</v>
       </c>
       <c r="G38" t="s">
         <v>40</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="K38" t="s">
         <v>11</v>
@@ -7092,18 +7092,18 @@
         <v>0305_Sol2 Str Heat</v>
       </c>
       <c r="Q38" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="R38" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q38,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q38,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0025</v>
       </c>
       <c r="T38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Imported Electricity','0025']</v>
       </c>
       <c r="U38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Imported Electricity':'0025',</v>
       </c>
     </row>
@@ -7121,20 +7121,20 @@
         <v>39</v>
       </c>
       <c r="E39" t="str">
-        <f>TRIM(C39) &amp;" " &amp; TRIM(D39)</f>
+        <f t="shared" si="3"/>
         <v>Storage2 Heat</v>
       </c>
       <c r="F39" t="s">
         <v>557</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I39" s="10">
         <v>11</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="K39" t="s">
         <v>11</v>
@@ -7164,11 +7164,11 @@
         <v>1800</v>
       </c>
       <c r="T39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Individual Electricity','1800']</v>
       </c>
       <c r="U39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Individual Electricity':'1800',</v>
       </c>
     </row>
@@ -7186,20 +7186,20 @@
         <v>39</v>
       </c>
       <c r="E40" t="str">
-        <f>TRIM(C40) &amp;" " &amp; TRIM(D40)</f>
+        <f t="shared" si="3"/>
         <v>Balance2 Heat</v>
       </c>
       <c r="F40" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I40" s="10">
         <v>12</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="K40" t="s">
         <v>11</v>
@@ -7229,11 +7229,11 @@
         <v>1700</v>
       </c>
       <c r="T40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Individual Heat 1','1700']</v>
       </c>
       <c r="U40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Individual Heat 1':'1700',</v>
       </c>
     </row>
@@ -7251,20 +7251,20 @@
         <v>39</v>
       </c>
       <c r="E41" t="str">
-        <f>TRIM(C41) &amp;" " &amp; TRIM(D41)</f>
+        <f t="shared" si="3"/>
         <v>CSHP 3 Heat</v>
       </c>
       <c r="G41" t="s">
         <v>42</v>
       </c>
       <c r="H41" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="I41" s="9" t="s">
         <v>584</v>
       </c>
-      <c r="I41" s="9" t="s">
-        <v>585</v>
-      </c>
       <c r="J41" s="10" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="K41" t="s">
         <v>11</v>
@@ -7294,11 +7294,11 @@
         <v>1900</v>
       </c>
       <c r="T41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Individual Heat 2','1900']</v>
       </c>
       <c r="U41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Individual Heat 2':'1900',</v>
       </c>
     </row>
@@ -7316,20 +7316,20 @@
         <v>39</v>
       </c>
       <c r="E42" t="str">
-        <f>TRIM(C42) &amp;" " &amp; TRIM(D42)</f>
+        <f t="shared" si="3"/>
         <v>Waste 3 Heat</v>
       </c>
       <c r="G42" t="s">
         <v>42</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="K42" t="s">
         <v>11</v>
@@ -7359,11 +7359,11 @@
         <v>1500</v>
       </c>
       <c r="T42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Market Prices','1500']</v>
       </c>
       <c r="U42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Market Prices':'1500',</v>
       </c>
     </row>
@@ -7381,20 +7381,20 @@
         <v>39</v>
       </c>
       <c r="E43" t="str">
-        <f>TRIM(C43) &amp;" " &amp; TRIM(D43)</f>
+        <f t="shared" si="3"/>
         <v>Geoth 3 Heat</v>
       </c>
       <c r="G43" t="s">
         <v>51</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="K43" t="s">
         <v>11</v>
@@ -7424,11 +7424,11 @@
         <v>1400</v>
       </c>
       <c r="T43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Nordpool Prices','1400']</v>
       </c>
       <c r="U43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Nordpool Prices':'1400',</v>
       </c>
     </row>
@@ -7446,20 +7446,20 @@
         <v>52</v>
       </c>
       <c r="E44" t="str">
-        <f>TRIM(C44) &amp;" " &amp; TRIM(D44)</f>
+        <f t="shared" si="3"/>
         <v>Geoth 3 Steam</v>
       </c>
       <c r="G44" t="s">
         <v>51</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K44" t="s">
         <v>11</v>
@@ -7489,11 +7489,11 @@
         <v>0700</v>
       </c>
       <c r="T44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Nuclear','0700']</v>
       </c>
       <c r="U44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Nuclear':'0700',</v>
       </c>
     </row>
@@ -7511,20 +7511,20 @@
         <v>53</v>
       </c>
       <c r="E45" t="str">
-        <f>TRIM(C45) &amp;" " &amp; TRIM(D45)</f>
+        <f t="shared" si="3"/>
         <v>Geoth 3 Storage</v>
       </c>
       <c r="G45" t="s">
         <v>51</v>
       </c>
       <c r="H45" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="I45" s="9" t="s">
         <v>585</v>
       </c>
-      <c r="I45" s="9" t="s">
-        <v>586</v>
-      </c>
       <c r="J45" s="10" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K45" t="s">
         <v>11</v>
@@ -7554,11 +7554,11 @@
         <v>0600</v>
       </c>
       <c r="T45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Power Plants Electricity Production','0600']</v>
       </c>
       <c r="U45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Power Plants Electricity Production':'0600',</v>
       </c>
     </row>
@@ -7576,20 +7576,20 @@
         <v>39</v>
       </c>
       <c r="E46" t="str">
-        <f>TRIM(C46) &amp;" " &amp; TRIM(D46)</f>
+        <f t="shared" si="3"/>
         <v>CHP 3 Heat</v>
       </c>
       <c r="F46" t="s">
         <v>553</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I46" s="10">
         <v>13</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="K46" t="s">
         <v>11</v>
@@ -7619,11 +7619,11 @@
         <v>0800</v>
       </c>
       <c r="T46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Pump Consumption','0800']</v>
       </c>
       <c r="U46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Pump Consumption':'0800',</v>
       </c>
     </row>
@@ -7641,20 +7641,20 @@
         <v>39</v>
       </c>
       <c r="E47" t="str">
-        <f>TRIM(C47) &amp;" " &amp; TRIM(D47)</f>
+        <f t="shared" si="3"/>
         <v>HP 3 Heat</v>
       </c>
       <c r="F47" t="s">
         <v>558</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I47" s="10">
         <v>14</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="K47" t="s">
         <v>11</v>
@@ -7684,11 +7684,11 @@
         <v>1000</v>
       </c>
       <c r="T47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Pump Storage','1000']</v>
       </c>
       <c r="U47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Pump Storage':'1000',</v>
       </c>
     </row>
@@ -7706,20 +7706,20 @@
         <v>39</v>
       </c>
       <c r="E48" t="str">
-        <f>TRIM(C48) &amp;" " &amp; TRIM(D48)</f>
+        <f t="shared" si="3"/>
         <v>Boiler 3 Heat</v>
       </c>
       <c r="F48" t="s">
         <v>68</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I48" s="10">
         <v>15</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="K48" t="s">
         <v>11</v>
@@ -7749,11 +7749,11 @@
         <v>0100</v>
       </c>
       <c r="T48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Renewable Energy Sources','0100']</v>
       </c>
       <c r="U48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Renewable Energy Sources':'0100',</v>
       </c>
     </row>
@@ -7771,20 +7771,20 @@
         <v>39</v>
       </c>
       <c r="E49" t="str">
-        <f>TRIM(C49) &amp;" " &amp; TRIM(D49)</f>
+        <f t="shared" si="3"/>
         <v>EH 3 Heat</v>
       </c>
       <c r="F49" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I49" s="10">
         <v>16</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="K49" t="s">
         <v>11</v>
@@ -7807,18 +7807,18 @@
         <v>0016_EH 3 Heat</v>
       </c>
       <c r="Q49" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="R49" t="str">
         <f>_xlfn.IFNA(VLOOKUP(Q49,Table1[[Full String]:[Serial]],5,0),VLOOKUP(Q49,Table1[[Parent]:[Serial]],2,0)&amp;"00")</f>
         <v>0024</v>
       </c>
       <c r="T49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Satbelization Load Percaentage','0024']</v>
       </c>
       <c r="U49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Satbelization Load Percaentage':'0024',</v>
       </c>
     </row>
@@ -7836,20 +7836,20 @@
         <v>39</v>
       </c>
       <c r="E50" t="str">
-        <f>TRIM(C50) &amp;" " &amp; TRIM(D50)</f>
+        <f t="shared" si="3"/>
         <v>ELT 3 Heat</v>
       </c>
       <c r="F50" t="s">
         <v>559</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I50" s="10">
         <v>17</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="K50" t="s">
         <v>11</v>
@@ -7879,11 +7879,11 @@
         <v>0300</v>
       </c>
       <c r="T50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Solar Thermal Powers','0300']</v>
       </c>
       <c r="U50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Solar Thermal Powers':'0300',</v>
       </c>
     </row>
@@ -7901,20 +7901,20 @@
         <v>72</v>
       </c>
       <c r="E51" t="str">
-        <f>TRIM(C51) &amp;" " &amp; TRIM(D51)</f>
+        <f t="shared" si="3"/>
         <v>Solar3 Heat</v>
       </c>
       <c r="G51" t="s">
         <v>40</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="K51" t="s">
         <v>11</v>
@@ -7944,11 +7944,11 @@
         <v>0011</v>
       </c>
       <c r="T51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Storage 2','0011']</v>
       </c>
       <c r="U51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Storage 2':'0011',</v>
       </c>
     </row>
@@ -7966,20 +7966,20 @@
         <v>39</v>
       </c>
       <c r="E52" t="str">
-        <f>TRIM(C52) &amp;" " &amp; TRIM(D52)</f>
+        <f t="shared" si="3"/>
         <v>Sol3 Str Heat</v>
       </c>
       <c r="G52" t="s">
         <v>40</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="K52" t="s">
         <v>11</v>
@@ -8009,11 +8009,11 @@
         <v>0018</v>
       </c>
       <c r="T52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Storage 3','0018']</v>
       </c>
       <c r="U52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Storage 3':'0018',</v>
       </c>
     </row>
@@ -8031,20 +8031,20 @@
         <v>39</v>
       </c>
       <c r="E53" t="str">
-        <f>TRIM(C53) &amp;" " &amp; TRIM(D53)</f>
+        <f t="shared" si="3"/>
         <v>Storage3 Heat</v>
       </c>
       <c r="F53" t="s">
         <v>555</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I53" s="10">
         <v>18</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="K53" t="s">
         <v>11</v>
@@ -8074,11 +8074,11 @@
         <v>2000</v>
       </c>
       <c r="T53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Transports Heat 2','2000']</v>
       </c>
       <c r="U53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Transports Heat 2':'2000',</v>
       </c>
     </row>
@@ -8096,20 +8096,20 @@
         <v>39</v>
       </c>
       <c r="E54" t="str">
-        <f>TRIM(C54) &amp;" " &amp; TRIM(D54)</f>
+        <f t="shared" si="3"/>
         <v>Balance3 Heat</v>
       </c>
       <c r="F54" t="s">
-        <v>560</v>
+        <v>739</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I54" s="10">
         <v>19</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="K54" t="s">
         <v>11</v>
@@ -8125,7 +8125,7 @@
       </c>
       <c r="O54" t="str">
         <f>Table1[[#This Row],[Serial]]&amp;(IF(ISBLANK(Table1[[#This Row],[Full String]]),Table1[[#This Row],[Parent]],Table1[[#This Row],[Full String]]))</f>
-        <v>0019Heat BalanceGgr.3</v>
+        <v>0019Heat Balance Gr.3</v>
       </c>
       <c r="P54" t="str">
         <f>Table1[[#This Row],[Serial]]&amp;"_"&amp;Table1[[#This Row],[String]]</f>
@@ -8139,11 +8139,11 @@
         <v>0900</v>
       </c>
       <c r="T54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>['Turbine Production','0900']</v>
       </c>
       <c r="U54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'Turbine Production':'0900',</v>
       </c>
     </row>
@@ -8161,20 +8161,20 @@
         <v>21</v>
       </c>
       <c r="E55" t="str">
-        <f>TRIM(C55) &amp;" " &amp; TRIM(D55)</f>
+        <f t="shared" si="3"/>
         <v>Flexible Electr.</v>
       </c>
       <c r="F55" t="s">
         <v>554</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I55" s="10">
         <v>20</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="K55" t="s">
         <v>11</v>
@@ -8211,20 +8211,20 @@
         <v>21</v>
       </c>
       <c r="E56" t="str">
-        <f>TRIM(C56) &amp;" " &amp; TRIM(D56)</f>
+        <f t="shared" si="3"/>
         <v>HP Electr.</v>
       </c>
       <c r="F56" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I56" s="10">
         <v>21</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="K56" t="s">
         <v>11</v>
@@ -8261,20 +8261,20 @@
         <v>21</v>
       </c>
       <c r="E57" t="str">
-        <f>TRIM(C57) &amp;" " &amp; TRIM(D57)</f>
+        <f t="shared" si="3"/>
         <v>CSHP Electr.</v>
       </c>
       <c r="F57" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I57" s="10">
         <v>22</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="K57" t="s">
         <v>11</v>
@@ -8311,20 +8311,20 @@
         <v>21</v>
       </c>
       <c r="E58" t="str">
-        <f>TRIM(C58) &amp;" " &amp; TRIM(D58)</f>
+        <f t="shared" si="3"/>
         <v>CHP Electr.</v>
       </c>
       <c r="F58" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I58" s="10">
         <v>23</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="K58" t="s">
         <v>11</v>
@@ -8361,20 +8361,20 @@
         <v>21</v>
       </c>
       <c r="E59" t="str">
-        <f>TRIM(C59) &amp;" " &amp; TRIM(D59)</f>
+        <f t="shared" si="3"/>
         <v>PP Electr.</v>
       </c>
       <c r="G59" t="s">
         <v>81</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="K59" t="s">
         <v>11</v>
@@ -8411,20 +8411,20 @@
         <v>21</v>
       </c>
       <c r="E60" t="str">
-        <f>TRIM(C60) &amp;" " &amp; TRIM(D60)</f>
+        <f t="shared" si="3"/>
         <v>PP2 Electr.</v>
       </c>
       <c r="G60" t="s">
         <v>81</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="K60" t="s">
         <v>11</v>
@@ -8461,20 +8461,20 @@
         <v>21</v>
       </c>
       <c r="E61" t="str">
-        <f>TRIM(C61) &amp;" " &amp; TRIM(D61)</f>
+        <f t="shared" si="3"/>
         <v>Nuclear Electr.</v>
       </c>
       <c r="G61" t="s">
         <v>84</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I61" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="K61" t="s">
         <v>11</v>
@@ -8511,20 +8511,20 @@
         <v>21</v>
       </c>
       <c r="E62" t="str">
-        <f>TRIM(C62) &amp;" " &amp; TRIM(D62)</f>
+        <f t="shared" si="3"/>
         <v>Geother. Electr.</v>
       </c>
       <c r="G62" t="s">
         <v>84</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I62" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="K62" t="s">
         <v>11</v>
@@ -8561,20 +8561,20 @@
         <v>21</v>
       </c>
       <c r="E63" t="str">
-        <f>TRIM(C63) &amp;" " &amp; TRIM(D63)</f>
+        <f t="shared" si="3"/>
         <v>Pump Electr.</v>
       </c>
       <c r="G63" t="s">
         <v>87</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I63" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K63" t="s">
         <v>11</v>
@@ -8611,20 +8611,20 @@
         <v>21</v>
       </c>
       <c r="E64" t="str">
-        <f>TRIM(C64) &amp;" " &amp; TRIM(D64)</f>
+        <f t="shared" si="3"/>
         <v>Turbine Electr.</v>
       </c>
       <c r="G64" t="s">
         <v>89</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="K64" t="s">
         <v>11</v>
@@ -8661,7 +8661,7 @@
         <v>53</v>
       </c>
       <c r="E65" t="str">
-        <f>TRIM(C65) &amp;" " &amp; TRIM(D65)</f>
+        <f t="shared" si="3"/>
         <v>Pumped Storage</v>
       </c>
       <c r="G65" t="s">
@@ -8671,10 +8671,10 @@
         <v>10</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="K65" t="s">
         <v>11</v>
@@ -8711,20 +8711,20 @@
         <v>21</v>
       </c>
       <c r="E66" t="str">
-        <f>TRIM(C66) &amp;" " &amp; TRIM(D66)</f>
+        <f t="shared" ref="E66:E97" si="4">TRIM(C66) &amp;" " &amp; TRIM(D66)</f>
         <v>Pump2 Electr.</v>
       </c>
       <c r="G66" t="s">
         <v>87</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I66" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="K66" t="s">
         <v>11</v>
@@ -8761,20 +8761,20 @@
         <v>21</v>
       </c>
       <c r="E67" t="str">
-        <f>TRIM(C67) &amp;" " &amp; TRIM(D67)</f>
+        <f t="shared" si="4"/>
         <v>Turbine2 Electr.</v>
       </c>
       <c r="G67" t="s">
         <v>89</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I67" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K67" t="s">
         <v>11</v>
@@ -8811,7 +8811,7 @@
         <v>53</v>
       </c>
       <c r="E68" t="str">
-        <f>TRIM(C68) &amp;" " &amp; TRIM(D68)</f>
+        <f t="shared" si="4"/>
         <v>Pumped2 Storage</v>
       </c>
       <c r="G68" t="s">
@@ -8821,10 +8821,10 @@
         <v>10</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="K68" t="s">
         <v>11</v>
@@ -8861,20 +8861,20 @@
         <v>21</v>
       </c>
       <c r="E69" t="str">
-        <f>TRIM(C69) &amp;" " &amp; TRIM(D69)</f>
+        <f t="shared" si="4"/>
         <v>Rock in Electr.</v>
       </c>
       <c r="G69" t="s">
         <v>89</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I69" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="K69" t="s">
         <v>11</v>
@@ -8911,20 +8911,20 @@
         <v>52</v>
       </c>
       <c r="E70" t="str">
-        <f>TRIM(C70) &amp;" " &amp; TRIM(D70)</f>
+        <f t="shared" si="4"/>
         <v>Rock out Steam</v>
       </c>
       <c r="G70" t="s">
         <v>89</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I70" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="K70" t="s">
         <v>11</v>
@@ -8961,20 +8961,20 @@
         <v>30</v>
       </c>
       <c r="E71" t="str">
-        <f>TRIM(C71) &amp;" " &amp; TRIM(D71)</f>
+        <f t="shared" si="4"/>
         <v>Rock str Storage</v>
       </c>
       <c r="G71" t="s">
         <v>89</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="K71" t="s">
         <v>11</v>
@@ -9011,20 +9011,20 @@
         <v>21</v>
       </c>
       <c r="E72" t="str">
-        <f>TRIM(C72) &amp;" " &amp; TRIM(D72)</f>
+        <f t="shared" si="4"/>
         <v>ELT 2 Electr.</v>
       </c>
       <c r="G72" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H72" s="10">
         <v>11</v>
       </c>
       <c r="I72" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="K72" t="s">
         <v>11</v>
@@ -9061,20 +9061,20 @@
         <v>99</v>
       </c>
       <c r="E73" t="str">
-        <f>TRIM(C73) &amp;" " &amp; TRIM(D73)</f>
+        <f t="shared" si="4"/>
         <v>ELT 2 H2 ELT 2</v>
       </c>
       <c r="G73" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H73" s="10">
         <v>11</v>
       </c>
       <c r="I73" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="K73" t="s">
         <v>11</v>
@@ -9111,20 +9111,20 @@
         <v>21</v>
       </c>
       <c r="E74" t="str">
-        <f>TRIM(C74) &amp;" " &amp; TRIM(D74)</f>
+        <f t="shared" si="4"/>
         <v>ELT 3 Electr.</v>
       </c>
       <c r="G74" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H74" s="10">
         <v>12</v>
       </c>
       <c r="I74" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="K74" t="s">
         <v>11</v>
@@ -9161,20 +9161,20 @@
         <v>101</v>
       </c>
       <c r="E75" t="str">
-        <f>TRIM(C75) &amp;" " &amp; TRIM(D75)</f>
+        <f t="shared" si="4"/>
         <v>ELT 3 H2 ELT 3</v>
       </c>
       <c r="G75" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H75" s="10">
         <v>12</v>
       </c>
       <c r="I75" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J75" s="10" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="K75" t="s">
         <v>11</v>
@@ -9211,7 +9211,7 @@
         <v>103</v>
       </c>
       <c r="E76" t="str">
-        <f>TRIM(C76) &amp;" " &amp; TRIM(D76)</f>
+        <f t="shared" si="4"/>
         <v>V2G Demand</v>
       </c>
       <c r="G76" t="s">
@@ -9221,10 +9221,10 @@
         <v>13</v>
       </c>
       <c r="I76" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="K76" t="s">
         <v>11</v>
@@ -9261,7 +9261,7 @@
         <v>105</v>
       </c>
       <c r="E77" t="str">
-        <f>TRIM(C77) &amp;" " &amp; TRIM(D77)</f>
+        <f t="shared" si="4"/>
         <v>V2G Charge</v>
       </c>
       <c r="G77" t="s">
@@ -9271,10 +9271,10 @@
         <v>13</v>
       </c>
       <c r="I77" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J77" s="10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="K77" t="s">
         <v>11</v>
@@ -9311,7 +9311,7 @@
         <v>106</v>
       </c>
       <c r="E78" t="str">
-        <f>TRIM(C78) &amp;" " &amp; TRIM(D78)</f>
+        <f t="shared" si="4"/>
         <v>V2G Discha.</v>
       </c>
       <c r="G78" t="s">
@@ -9321,10 +9321,10 @@
         <v>13</v>
       </c>
       <c r="I78" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J78" s="10" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="K78" t="s">
         <v>11</v>
@@ -9361,7 +9361,7 @@
         <v>30</v>
       </c>
       <c r="E79" t="str">
-        <f>TRIM(C79) &amp;" " &amp; TRIM(D79)</f>
+        <f t="shared" si="4"/>
         <v>V2G Storage</v>
       </c>
       <c r="G79" t="s">
@@ -9371,10 +9371,10 @@
         <v>13</v>
       </c>
       <c r="I79" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="K79" t="s">
         <v>11</v>
@@ -9411,7 +9411,7 @@
         <v>21</v>
       </c>
       <c r="E80" t="str">
-        <f>TRIM(C80) &amp;" " &amp; TRIM(D80)</f>
+        <f t="shared" si="4"/>
         <v>H2 Electr.</v>
       </c>
       <c r="G80" t="s">
@@ -9421,10 +9421,10 @@
         <v>20</v>
       </c>
       <c r="I80" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="K80" t="s">
         <v>11</v>
@@ -9461,7 +9461,7 @@
         <v>30</v>
       </c>
       <c r="E81" t="str">
-        <f>TRIM(C81) &amp;" " &amp; TRIM(D81)</f>
+        <f t="shared" si="4"/>
         <v>H2 Storage</v>
       </c>
       <c r="G81" t="s">
@@ -9471,10 +9471,10 @@
         <v>20</v>
       </c>
       <c r="I81" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J81" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="K81" t="s">
         <v>11</v>
@@ -9511,7 +9511,7 @@
         <v>21</v>
       </c>
       <c r="E82" t="str">
-        <f>TRIM(C82) &amp;" " &amp; TRIM(D82)</f>
+        <f t="shared" si="4"/>
         <v>CO2Hydro Electr.</v>
       </c>
       <c r="G82" t="s">
@@ -9521,10 +9521,10 @@
         <v>20</v>
       </c>
       <c r="I82" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="K82" t="s">
         <v>11</v>
@@ -9561,7 +9561,7 @@
         <v>21</v>
       </c>
       <c r="E83" t="str">
-        <f>TRIM(C83) &amp;" " &amp; TRIM(D83)</f>
+        <f t="shared" si="4"/>
         <v>NH3Hydro Electr.</v>
       </c>
       <c r="G83" t="s">
@@ -9571,10 +9571,10 @@
         <v>20</v>
       </c>
       <c r="I83" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K83" t="s">
         <v>11</v>
@@ -9611,7 +9611,7 @@
         <v>111</v>
       </c>
       <c r="E84" t="str">
-        <f>TRIM(C84) &amp;" " &amp; TRIM(D84)</f>
+        <f t="shared" si="4"/>
         <v>CO2Hydro liq.fuel</v>
       </c>
       <c r="G84" t="s">
@@ -9621,10 +9621,10 @@
         <v>20</v>
       </c>
       <c r="I84" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J84" s="10" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="K84" t="s">
         <v>11</v>
@@ -9661,7 +9661,7 @@
         <v>112</v>
       </c>
       <c r="E85" t="str">
-        <f>TRIM(C85) &amp;" " &amp; TRIM(D85)</f>
+        <f t="shared" si="4"/>
         <v>NH3Hydro Ammonia</v>
       </c>
       <c r="G85" t="s">
@@ -9671,10 +9671,10 @@
         <v>20</v>
       </c>
       <c r="I85" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="K85" t="s">
         <v>11</v>
@@ -9711,7 +9711,7 @@
         <v>21</v>
       </c>
       <c r="E86" t="str">
-        <f>TRIM(C86) &amp;" " &amp; TRIM(D86)</f>
+        <f t="shared" si="4"/>
         <v>HH-CHP Electr.</v>
       </c>
       <c r="G86" t="s">
@@ -9721,10 +9721,10 @@
         <v>18</v>
       </c>
       <c r="I86" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J86" s="10" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K86" t="s">
         <v>11</v>
@@ -9761,7 +9761,7 @@
         <v>21</v>
       </c>
       <c r="E87" t="str">
-        <f>TRIM(C87) &amp;" " &amp; TRIM(D87)</f>
+        <f t="shared" si="4"/>
         <v>HH-HP Electr.</v>
       </c>
       <c r="G87" t="s">
@@ -9771,10 +9771,10 @@
         <v>18</v>
       </c>
       <c r="I87" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J87" s="10" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="K87" t="s">
         <v>11</v>
@@ -9811,7 +9811,7 @@
         <v>21</v>
       </c>
       <c r="E88" t="str">
-        <f>TRIM(C88) &amp;" " &amp; TRIM(D88)</f>
+        <f t="shared" si="4"/>
         <v>HH-HP/EB Electr.</v>
       </c>
       <c r="G88" t="s">
@@ -9821,10 +9821,10 @@
         <v>18</v>
       </c>
       <c r="I88" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J88" s="10" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K88" t="s">
         <v>11</v>
@@ -9861,7 +9861,7 @@
         <v>21</v>
       </c>
       <c r="E89" t="str">
-        <f>TRIM(C89) &amp;" " &amp; TRIM(D89)</f>
+        <f t="shared" si="4"/>
         <v>HH-EB Electr.</v>
       </c>
       <c r="G89" t="s">
@@ -9871,10 +9871,10 @@
         <v>18</v>
       </c>
       <c r="I89" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J89" s="10" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K89" t="s">
         <v>11</v>
@@ -9911,7 +9911,7 @@
         <v>21</v>
       </c>
       <c r="E90" t="str">
-        <f>TRIM(C90) &amp;" " &amp; TRIM(D90)</f>
+        <f t="shared" si="4"/>
         <v>HH-H2 Electr.</v>
       </c>
       <c r="G90" t="s">
@@ -9921,10 +9921,10 @@
         <v>19</v>
       </c>
       <c r="I90" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J90" s="10" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K90" t="s">
         <v>11</v>
@@ -9961,7 +9961,7 @@
         <v>30</v>
       </c>
       <c r="E91" t="str">
-        <f>TRIM(C91) &amp;" " &amp; TRIM(D91)</f>
+        <f t="shared" si="4"/>
         <v>HH-H2 Storage</v>
       </c>
       <c r="G91" t="s">
@@ -9971,10 +9971,10 @@
         <v>19</v>
       </c>
       <c r="I91" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J91" s="10" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="K91" t="s">
         <v>11</v>
@@ -10011,7 +10011,7 @@
         <v>120</v>
       </c>
       <c r="E92" t="str">
-        <f>TRIM(C92) &amp;" " &amp; TRIM(D92)</f>
+        <f t="shared" si="4"/>
         <v>HH-H2 Prices</v>
       </c>
       <c r="G92" t="s">
@@ -10021,10 +10021,10 @@
         <v>19</v>
       </c>
       <c r="I92" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J92" s="10" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="K92" t="s">
         <v>11</v>
@@ -10061,7 +10061,7 @@
         <v>39</v>
       </c>
       <c r="E93" t="str">
-        <f>TRIM(C93) &amp;" " &amp; TRIM(D93)</f>
+        <f t="shared" si="4"/>
         <v>HH Dem. Heat</v>
       </c>
       <c r="G93" t="s">
@@ -10071,10 +10071,10 @@
         <v>17</v>
       </c>
       <c r="I93" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J93" s="10" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="K93" t="s">
         <v>11</v>
@@ -10111,7 +10111,7 @@
         <v>39</v>
       </c>
       <c r="E94" t="str">
-        <f>TRIM(C94) &amp;" " &amp; TRIM(D94)</f>
+        <f t="shared" si="4"/>
         <v>HH CHP+HP Heat</v>
       </c>
       <c r="G94" t="s">
@@ -10121,10 +10121,10 @@
         <v>17</v>
       </c>
       <c r="I94" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J94" s="10" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K94" t="s">
         <v>11</v>
@@ -10161,7 +10161,7 @@
         <v>39</v>
       </c>
       <c r="E95" t="str">
-        <f>TRIM(C95) &amp;" " &amp; TRIM(D95)</f>
+        <f t="shared" si="4"/>
         <v>HH Boil. Heat</v>
       </c>
       <c r="G95" t="s">
@@ -10171,10 +10171,10 @@
         <v>17</v>
       </c>
       <c r="I95" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J95" s="10" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="K95" t="s">
         <v>11</v>
@@ -10211,7 +10211,7 @@
         <v>39</v>
       </c>
       <c r="E96" t="str">
-        <f>TRIM(C96) &amp;" " &amp; TRIM(D96)</f>
+        <f t="shared" si="4"/>
         <v>HH Solar Heat</v>
       </c>
       <c r="G96" t="s">
@@ -10221,10 +10221,10 @@
         <v>17</v>
       </c>
       <c r="I96" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J96" s="10" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="K96" t="s">
         <v>11</v>
@@ -10261,7 +10261,7 @@
         <v>39</v>
       </c>
       <c r="E97" t="str">
-        <f>TRIM(C97) &amp;" " &amp; TRIM(D97)</f>
+        <f t="shared" si="4"/>
         <v>HH Store Heat</v>
       </c>
       <c r="G97" t="s">
@@ -10271,10 +10271,10 @@
         <v>17</v>
       </c>
       <c r="I97" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J97" s="10" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="K97" t="s">
         <v>11</v>
@@ -10311,7 +10311,7 @@
         <v>39</v>
       </c>
       <c r="E98" t="str">
-        <f>TRIM(C98) &amp;" " &amp; TRIM(D98)</f>
+        <f t="shared" ref="E98:E129" si="5">TRIM(C98) &amp;" " &amp; TRIM(D98)</f>
         <v>HH Balan Heat</v>
       </c>
       <c r="G98" t="s">
@@ -10321,10 +10321,10 @@
         <v>17</v>
       </c>
       <c r="I98" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J98" s="10" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="K98" t="s">
         <v>11</v>
@@ -10361,20 +10361,20 @@
         <v>129</v>
       </c>
       <c r="E99" t="str">
-        <f>TRIM(C99) &amp;" " &amp; TRIM(D99)</f>
+        <f t="shared" si="5"/>
         <v>Stabil. LoadPercent</v>
       </c>
       <c r="F99" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H99" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I99" s="10">
         <v>24</v>
       </c>
       <c r="J99" s="10" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="K99" t="s">
         <v>130</v>
@@ -10411,20 +10411,20 @@
         <v>21</v>
       </c>
       <c r="E100" t="str">
-        <f>TRIM(C100) &amp;" " &amp; TRIM(D100)</f>
+        <f t="shared" si="5"/>
         <v>Import Electr.</v>
       </c>
       <c r="F100" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H100" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I100" s="10">
         <v>25</v>
       </c>
       <c r="J100" s="10" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="K100" t="s">
         <v>11</v>
@@ -10461,20 +10461,20 @@
         <v>21</v>
       </c>
       <c r="E101" t="str">
-        <f>TRIM(C101) &amp;" " &amp; TRIM(D101)</f>
+        <f t="shared" si="5"/>
         <v>Export Electr.</v>
       </c>
       <c r="F101" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H101" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I101" s="10">
         <v>26</v>
       </c>
       <c r="J101" s="10" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="K101" t="s">
         <v>11</v>
@@ -10511,20 +10511,20 @@
         <v>21</v>
       </c>
       <c r="E102" t="str">
-        <f>TRIM(C102) &amp;" " &amp; TRIM(D102)</f>
+        <f t="shared" si="5"/>
         <v>CEEP Electr.</v>
       </c>
       <c r="F102" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H102" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I102" s="10">
         <v>27</v>
       </c>
       <c r="J102" s="10" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="K102" t="s">
         <v>11</v>
@@ -10561,20 +10561,20 @@
         <v>21</v>
       </c>
       <c r="E103" t="str">
-        <f>TRIM(C103) &amp;" " &amp; TRIM(D103)</f>
+        <f t="shared" si="5"/>
         <v>EEEP Electr.</v>
       </c>
       <c r="F103" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H103" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I103" s="10">
         <v>28</v>
       </c>
       <c r="J103" s="10" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="K103" t="s">
         <v>11</v>
@@ -10611,7 +10611,7 @@
         <v>120</v>
       </c>
       <c r="E104" t="str">
-        <f>TRIM(C104) &amp;" " &amp; TRIM(D104)</f>
+        <f t="shared" si="5"/>
         <v>ExMarket Prices</v>
       </c>
       <c r="G104" t="s">
@@ -10621,10 +10621,10 @@
         <v>14</v>
       </c>
       <c r="I104" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J104" s="10" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="K104" t="s">
         <v>11</v>
@@ -10661,7 +10661,7 @@
         <v>137</v>
       </c>
       <c r="E105" t="str">
-        <f>TRIM(C105) &amp;" " &amp; TRIM(D105)</f>
+        <f t="shared" si="5"/>
         <v>ExMarket Prod</v>
       </c>
       <c r="G105" t="s">
@@ -10671,10 +10671,10 @@
         <v>14</v>
       </c>
       <c r="I105" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J105" s="10" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="K105" t="s">
         <v>11</v>
@@ -10711,7 +10711,7 @@
         <v>120</v>
       </c>
       <c r="E106" t="str">
-        <f>TRIM(C106) &amp;" " &amp; TRIM(D106)</f>
+        <f t="shared" si="5"/>
         <v>System Prices</v>
       </c>
       <c r="G106" t="s">
@@ -10721,10 +10721,10 @@
         <v>15</v>
       </c>
       <c r="I106" s="11" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J106" s="12" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="K106" t="s">
         <v>11</v>
@@ -10761,7 +10761,7 @@
         <v>120</v>
       </c>
       <c r="E107" t="str">
-        <f>TRIM(C107) &amp;" " &amp; TRIM(D107)</f>
+        <f t="shared" si="5"/>
         <v>InMarket Prices</v>
       </c>
       <c r="G107" t="s">
@@ -10771,10 +10771,10 @@
         <v>15</v>
       </c>
       <c r="I107" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J107" s="10" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="K107" t="s">
         <v>11</v>
@@ -10811,7 +10811,7 @@
         <v>120</v>
       </c>
       <c r="E108" t="str">
-        <f>TRIM(C108) &amp;" " &amp; TRIM(D108)</f>
+        <f t="shared" si="5"/>
         <v>Btl-neck Prices</v>
       </c>
       <c r="G108" t="s">
@@ -10821,10 +10821,10 @@
         <v>15</v>
       </c>
       <c r="I108" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J108" s="10" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="K108" t="s">
         <v>11</v>
@@ -10861,20 +10861,20 @@
         <v>142</v>
       </c>
       <c r="E109" t="str">
-        <f>TRIM(C109) &amp;" " &amp; TRIM(D109)</f>
+        <f t="shared" si="5"/>
         <v>Import Payment</v>
       </c>
       <c r="F109" t="s">
         <v>311</v>
       </c>
       <c r="H109" s="11" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I109" s="12">
         <v>29</v>
       </c>
       <c r="J109" s="12" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="K109" t="s">
         <v>11</v>
@@ -10911,7 +10911,7 @@
         <v>142</v>
       </c>
       <c r="E110" t="str">
-        <f>TRIM(C110) &amp;" " &amp; TRIM(D110)</f>
+        <f t="shared" si="5"/>
         <v>Export Payment</v>
       </c>
       <c r="G110" t="s">
@@ -10921,10 +10921,10 @@
         <v>16</v>
       </c>
       <c r="I110" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J110" s="10" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="K110" t="s">
         <v>11</v>
@@ -10961,7 +10961,7 @@
         <v>142</v>
       </c>
       <c r="E111" t="str">
-        <f>TRIM(C111) &amp;" " &amp; TRIM(D111)</f>
+        <f t="shared" si="5"/>
         <v>Blt-neck Payment</v>
       </c>
       <c r="G111" t="s">
@@ -10971,10 +10971,10 @@
         <v>16</v>
       </c>
       <c r="I111" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J111" s="10" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="K111" t="s">
         <v>11</v>
@@ -11011,20 +11011,20 @@
         <v>142</v>
       </c>
       <c r="E112" t="str">
-        <f>TRIM(C112) &amp;" " &amp; TRIM(D112)</f>
+        <f t="shared" si="5"/>
         <v>Add-exp Payment</v>
       </c>
       <c r="F112" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H112" s="11" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I112" s="12">
         <v>30</v>
       </c>
       <c r="J112" s="12" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="K112" t="s">
         <v>11</v>
@@ -11061,7 +11061,7 @@
         <v>147</v>
       </c>
       <c r="E113" t="str">
-        <f>TRIM(C113) &amp;" " &amp; TRIM(D113)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Boilers </v>
       </c>
       <c r="G113" t="s">
@@ -11071,10 +11071,10 @@
         <v>23</v>
       </c>
       <c r="I113" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J113" s="10" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="K113" t="s">
         <v>11</v>
@@ -11111,7 +11111,7 @@
         <v>147</v>
       </c>
       <c r="E114" t="str">
-        <f>TRIM(C114) &amp;" " &amp; TRIM(D114)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">CHP2+3 </v>
       </c>
       <c r="G114" t="s">
@@ -11121,10 +11121,10 @@
         <v>23</v>
       </c>
       <c r="I114" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J114" s="10" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="K114" t="s">
         <v>11</v>
@@ -11161,7 +11161,7 @@
         <v>150</v>
       </c>
       <c r="E115" t="str">
-        <f>TRIM(C115) &amp;" " &amp; TRIM(D115)</f>
+        <f t="shared" si="5"/>
         <v>PP CAES</v>
       </c>
       <c r="G115" t="s">
@@ -11171,10 +11171,10 @@
         <v>23</v>
       </c>
       <c r="I115" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J115" s="10" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="K115" t="s">
         <v>11</v>
@@ -11211,7 +11211,7 @@
         <v>152</v>
       </c>
       <c r="E116" t="str">
-        <f>TRIM(C116) &amp;" " &amp; TRIM(D116)</f>
+        <f t="shared" si="5"/>
         <v>Indi- vidual</v>
       </c>
       <c r="G116" t="s">
@@ -11221,10 +11221,10 @@
         <v>23</v>
       </c>
       <c r="I116" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J116" s="10" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="K116" t="s">
         <v>11</v>
@@ -11261,7 +11261,7 @@
         <v>147</v>
       </c>
       <c r="E117" t="str">
-        <f>TRIM(C117) &amp;" " &amp; TRIM(D117)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Transp. </v>
       </c>
       <c r="G117" t="s">
@@ -11271,10 +11271,10 @@
         <v>23</v>
       </c>
       <c r="I117" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J117" s="10" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K117" t="s">
         <v>11</v>
@@ -11311,7 +11311,7 @@
         <v>155</v>
       </c>
       <c r="E118" t="str">
-        <f>TRIM(C118) &amp;" " &amp; TRIM(D118)</f>
+        <f t="shared" si="5"/>
         <v>Indust. Various</v>
       </c>
       <c r="G118" t="s">
@@ -11321,10 +11321,10 @@
         <v>23</v>
       </c>
       <c r="I118" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J118" s="10" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="K118" t="s">
         <v>11</v>
@@ -11361,7 +11361,7 @@
         <v>156</v>
       </c>
       <c r="E119" t="str">
-        <f>TRIM(C119) &amp;" " &amp; TRIM(D119)</f>
+        <f t="shared" si="5"/>
         <v>Demand Sum</v>
       </c>
       <c r="G119" t="s">
@@ -11371,10 +11371,10 @@
         <v>23</v>
       </c>
       <c r="I119" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J119" s="10" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="K119" t="s">
         <v>11</v>
@@ -11411,7 +11411,7 @@
         <v>147</v>
       </c>
       <c r="E120" t="str">
-        <f>TRIM(C120) &amp;" " &amp; TRIM(D120)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Biogas </v>
       </c>
       <c r="G120" t="s">
@@ -11421,10 +11421,10 @@
         <v>23</v>
       </c>
       <c r="I120" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J120" s="10" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="K120" t="s">
         <v>11</v>
@@ -11461,7 +11461,7 @@
         <v>147</v>
       </c>
       <c r="E121" t="str">
-        <f>TRIM(C121) &amp;" " &amp; TRIM(D121)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Syngas </v>
       </c>
       <c r="G121" t="s">
@@ -11471,10 +11471,10 @@
         <v>23</v>
       </c>
       <c r="I121" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J121" s="10" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="K121" t="s">
         <v>11</v>
@@ -11511,7 +11511,7 @@
         <v>147</v>
       </c>
       <c r="E122" t="str">
-        <f>TRIM(C122) &amp;" " &amp; TRIM(D122)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">CO2HyGas </v>
       </c>
       <c r="G122" t="s">
@@ -11524,7 +11524,7 @@
         <v>10</v>
       </c>
       <c r="J122" s="10" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="K122" t="s">
         <v>11</v>
@@ -11561,7 +11561,7 @@
         <v>147</v>
       </c>
       <c r="E123" t="str">
-        <f>TRIM(C123) &amp;" " &amp; TRIM(D123)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">SynHyGas </v>
       </c>
       <c r="G123" t="s">
@@ -11574,7 +11574,7 @@
         <v>11</v>
       </c>
       <c r="J123" s="10" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="K123" t="s">
         <v>11</v>
@@ -11611,7 +11611,7 @@
         <v>147</v>
       </c>
       <c r="E124" t="str">
-        <f>TRIM(C124) &amp;" " &amp; TRIM(D124)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">SynFuel </v>
       </c>
       <c r="G124" t="s">
@@ -11624,7 +11624,7 @@
         <v>12</v>
       </c>
       <c r="J124" s="10" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="K124" t="s">
         <v>11</v>
@@ -11661,7 +11661,7 @@
         <v>147</v>
       </c>
       <c r="E125" t="str">
-        <f>TRIM(C125) &amp;" " &amp; TRIM(D125)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Storage </v>
       </c>
       <c r="G125" t="s">
@@ -11674,7 +11674,7 @@
         <v>13</v>
       </c>
       <c r="J125" s="10" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="K125" t="s">
         <v>11</v>
@@ -11711,7 +11711,7 @@
         <v>162</v>
       </c>
       <c r="E126" t="str">
-        <f>TRIM(C126) &amp;" " &amp; TRIM(D126)</f>
+        <f t="shared" si="5"/>
         <v>Storage Content</v>
       </c>
       <c r="G126" t="s">
@@ -11724,7 +11724,7 @@
         <v>14</v>
       </c>
       <c r="J126" s="10" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="K126" t="s">
         <v>11</v>
@@ -11761,7 +11761,7 @@
         <v>147</v>
       </c>
       <c r="E127" t="str">
-        <f>TRIM(C127) &amp;" " &amp; TRIM(D127)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">Sum </v>
       </c>
       <c r="G127" t="s">
@@ -11774,7 +11774,7 @@
         <v>15</v>
       </c>
       <c r="J127" s="10" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="K127" t="s">
         <v>11</v>
@@ -11811,7 +11811,7 @@
         <v>164</v>
       </c>
       <c r="E128" t="str">
-        <f>TRIM(C128) &amp;" " &amp; TRIM(D128)</f>
+        <f t="shared" si="5"/>
         <v>Import Gas</v>
       </c>
       <c r="G128" t="s">
@@ -11824,7 +11824,7 @@
         <v>16</v>
       </c>
       <c r="J128" s="10" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="K128" t="s">
         <v>11</v>
@@ -11861,7 +11861,7 @@
         <v>164</v>
       </c>
       <c r="E129" t="str">
-        <f>TRIM(C129) &amp;" " &amp; TRIM(D129)</f>
+        <f t="shared" si="5"/>
         <v>Export Gas</v>
       </c>
       <c r="G129" t="s">
@@ -11874,7 +11874,7 @@
         <v>17</v>
       </c>
       <c r="J129" s="10" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="K129" t="s">
         <v>11</v>
@@ -11911,7 +11911,7 @@
         <v>103</v>
       </c>
       <c r="E130" t="str">
-        <f>TRIM(C130) &amp;" " &amp; TRIM(D130)</f>
+        <f t="shared" ref="E130:E161" si="6">TRIM(C130) &amp;" " &amp; TRIM(D130)</f>
         <v>FreshW Demand</v>
       </c>
       <c r="G130" t="s">
@@ -11921,10 +11921,10 @@
         <v>22</v>
       </c>
       <c r="I130" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J130" s="10" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="K130" t="s">
         <v>11</v>
@@ -11961,7 +11961,7 @@
         <v>30</v>
       </c>
       <c r="E131" t="str">
-        <f>TRIM(C131) &amp;" " &amp; TRIM(D131)</f>
+        <f t="shared" si="6"/>
         <v>FreshW Storage</v>
       </c>
       <c r="G131" t="s">
@@ -11971,10 +11971,10 @@
         <v>22</v>
       </c>
       <c r="I131" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J131" s="10" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="K131" t="s">
         <v>11</v>
@@ -12011,7 +12011,7 @@
         <v>103</v>
       </c>
       <c r="E132" t="str">
-        <f>TRIM(C132) &amp;" " &amp; TRIM(D132)</f>
+        <f t="shared" si="6"/>
         <v>SaltW Demand</v>
       </c>
       <c r="G132" t="s">
@@ -12021,10 +12021,10 @@
         <v>22</v>
       </c>
       <c r="I132" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J132" s="10" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="K132" t="s">
         <v>11</v>
@@ -12061,7 +12061,7 @@
         <v>169</v>
       </c>
       <c r="E133" t="str">
-        <f>TRIM(C133) &amp;" " &amp; TRIM(D133)</f>
+        <f t="shared" si="6"/>
         <v>Brine Prod.</v>
       </c>
       <c r="G133" t="s">
@@ -12071,10 +12071,10 @@
         <v>22</v>
       </c>
       <c r="I133" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J133" s="10" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="K133" t="s">
         <v>11</v>
@@ -12111,7 +12111,7 @@
         <v>30</v>
       </c>
       <c r="E134" t="str">
-        <f>TRIM(C134) &amp;" " &amp; TRIM(D134)</f>
+        <f t="shared" si="6"/>
         <v>Brine Storage</v>
       </c>
       <c r="G134" t="s">
@@ -12121,10 +12121,10 @@
         <v>22</v>
       </c>
       <c r="I134" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J134" s="10" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="K134" t="s">
         <v>11</v>
@@ -12161,7 +12161,7 @@
         <v>21</v>
       </c>
       <c r="E135" t="str">
-        <f>TRIM(C135) &amp;" " &amp; TRIM(D135)</f>
+        <f t="shared" si="6"/>
         <v>Desal.Pl Electr.</v>
       </c>
       <c r="G135" t="s">
@@ -12171,10 +12171,10 @@
         <v>22</v>
       </c>
       <c r="I135" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J135" s="10" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="K135" t="s">
         <v>11</v>
@@ -12211,7 +12211,7 @@
         <v>21</v>
       </c>
       <c r="E136" t="str">
-        <f>TRIM(C136) &amp;" " &amp; TRIM(D136)</f>
+        <f t="shared" si="6"/>
         <v>FWPump Electr.</v>
       </c>
       <c r="G136" t="s">
@@ -12221,10 +12221,10 @@
         <v>22</v>
       </c>
       <c r="I136" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J136" s="10" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="K136" t="s">
         <v>11</v>
@@ -12261,7 +12261,7 @@
         <v>21</v>
       </c>
       <c r="E137" t="str">
-        <f>TRIM(C137) &amp;" " &amp; TRIM(D137)</f>
+        <f t="shared" si="6"/>
         <v>Turbine Electr.</v>
       </c>
       <c r="G137" t="s">
@@ -12271,10 +12271,10 @@
         <v>22</v>
       </c>
       <c r="I137" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J137" s="10" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="K137" t="s">
         <v>11</v>
@@ -12311,7 +12311,7 @@
         <v>21</v>
       </c>
       <c r="E138" t="str">
-        <f>TRIM(C138) &amp;" " &amp; TRIM(D138)</f>
+        <f t="shared" si="6"/>
         <v>Pump Electr.</v>
       </c>
       <c r="G138" t="s">
@@ -12321,10 +12321,10 @@
         <v>22</v>
       </c>
       <c r="I138" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J138" s="10" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="K138" t="s">
         <v>11</v>
@@ -12361,7 +12361,7 @@
         <v>103</v>
       </c>
       <c r="E139" t="str">
-        <f>TRIM(C139) &amp;" " &amp; TRIM(D139)</f>
+        <f t="shared" si="6"/>
         <v>CoolGr1 Demand</v>
       </c>
       <c r="G139" t="s">
@@ -12371,10 +12371,10 @@
         <v>21</v>
       </c>
       <c r="I139" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J139" s="10" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="K139" t="s">
         <v>11</v>
@@ -12411,7 +12411,7 @@
         <v>103</v>
       </c>
       <c r="E140" t="str">
-        <f>TRIM(C140) &amp;" " &amp; TRIM(D140)</f>
+        <f t="shared" si="6"/>
         <v>CoolGr2 Demand</v>
       </c>
       <c r="G140" t="s">
@@ -12421,10 +12421,10 @@
         <v>21</v>
       </c>
       <c r="I140" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J140" s="10" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="K140" t="s">
         <v>11</v>
@@ -12461,7 +12461,7 @@
         <v>103</v>
       </c>
       <c r="E141" t="str">
-        <f>TRIM(C141) &amp;" " &amp; TRIM(D141)</f>
+        <f t="shared" si="6"/>
         <v>CoolGr3 Demand</v>
       </c>
       <c r="G141" t="s">
@@ -12471,10 +12471,10 @@
         <v>21</v>
       </c>
       <c r="I141" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J141" s="10" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="K141" t="s">
         <v>11</v>
@@ -12511,7 +12511,7 @@
         <v>103</v>
       </c>
       <c r="E142" t="str">
-        <f>TRIM(C142) &amp;" " &amp; TRIM(D142)</f>
+        <f t="shared" si="6"/>
         <v>Cool-El Demand</v>
       </c>
       <c r="G142" t="s">
@@ -12521,10 +12521,10 @@
         <v>21</v>
       </c>
       <c r="I142" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J142" s="10" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="K142" t="s">
         <v>11</v>
@@ -12561,7 +12561,7 @@
         <v>177</v>
       </c>
       <c r="E143" t="str">
-        <f>TRIM(C143) &amp;" " &amp; TRIM(D143)</f>
+        <f t="shared" si="6"/>
         <v>CoolGr1 Natural</v>
       </c>
       <c r="G143" t="s">
@@ -12571,10 +12571,10 @@
         <v>21</v>
       </c>
       <c r="I143" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J143" s="10" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="K143" t="s">
         <v>11</v>
@@ -12611,7 +12611,7 @@
         <v>177</v>
       </c>
       <c r="E144" t="str">
-        <f>TRIM(C144) &amp;" " &amp; TRIM(D144)</f>
+        <f t="shared" si="6"/>
         <v>CoolGr2 Natural</v>
       </c>
       <c r="G144" t="s">
@@ -12621,10 +12621,10 @@
         <v>21</v>
       </c>
       <c r="I144" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J144" s="10" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="K144" t="s">
         <v>11</v>
@@ -12661,7 +12661,7 @@
         <v>177</v>
       </c>
       <c r="E145" t="str">
-        <f>TRIM(C145) &amp;" " &amp; TRIM(D145)</f>
+        <f t="shared" si="6"/>
         <v>CoolGr3 Natural</v>
       </c>
       <c r="G145" t="s">
@@ -12671,10 +12671,10 @@
         <v>21</v>
       </c>
       <c r="I145" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J145" s="10" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="K145" t="s">
         <v>11</v>
@@ -12711,7 +12711,7 @@
         <v>179</v>
       </c>
       <c r="E146" t="str">
-        <f>TRIM(C146) &amp;" " &amp; TRIM(D146)</f>
+        <f t="shared" si="6"/>
         <v>Cooling DHgr1</v>
       </c>
       <c r="G146" t="s">
@@ -12721,10 +12721,10 @@
         <v>21</v>
       </c>
       <c r="I146" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J146" s="10" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K146" t="s">
         <v>11</v>
@@ -12761,7 +12761,7 @@
         <v>180</v>
       </c>
       <c r="E147" t="str">
-        <f>TRIM(C147) &amp;" " &amp; TRIM(D147)</f>
+        <f t="shared" si="6"/>
         <v>Cooling DHgr2</v>
       </c>
       <c r="G147" t="s">
@@ -12771,10 +12771,10 @@
         <v>21</v>
       </c>
       <c r="I147" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J147" s="10" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="K147" t="s">
         <v>11</v>
@@ -12811,7 +12811,7 @@
         <v>181</v>
       </c>
       <c r="E148" t="str">
-        <f>TRIM(C148) &amp;" " &amp; TRIM(D148)</f>
+        <f t="shared" si="6"/>
         <v>Cooling DHgr3</v>
       </c>
       <c r="G148" t="s">
@@ -12824,7 +12824,7 @@
         <v>10</v>
       </c>
       <c r="J148" s="10" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="K148" t="s">
         <v>11</v>
@@ -12861,7 +12861,7 @@
         <v>21</v>
       </c>
       <c r="E149" t="str">
-        <f>TRIM(C149) &amp;" " &amp; TRIM(D149)</f>
+        <f t="shared" si="6"/>
         <v>Cooling Electr.</v>
       </c>
       <c r="G149" t="s">
@@ -12874,7 +12874,7 @@
         <v>11</v>
       </c>
       <c r="J149" s="10" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="K149" t="s">
         <v>11</v>

</xml_diff>